<commit_message>
made product supplier relation many to many
</commit_message>
<xml_diff>
--- a/AmpedBiz/.data/ImportFiles/Nicon/default_suppliers.xlsx
+++ b/AmpedBiz/.data/ImportFiles/Nicon/default_suppliers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Narasoft\tinda\trunk\AmpedBiz\AmpedBiz.Service.Host\Data\Default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Narasoft\tinda\trunk\AmpedBiz\.data\ImportFiles\Nicon\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">smscci_coffee!$A$2:$O$42</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">smscci_coffee!$1:$8</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>SAN MIGUEL INTEGRATED SALES</t>
   </si>
@@ -414,19 +414,25 @@
     <t>SRP/TP</t>
   </si>
   <si>
-    <t>Supplier Name</t>
-  </si>
-  <si>
     <t>SMIS</t>
   </si>
   <si>
-    <t>Supplier Id</t>
-  </si>
-  <si>
     <t>SAN MIGUEL</t>
   </si>
   <si>
     <t>Contact Person</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>ANOTHER SUPPLIER</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -2831,10 +2837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2857,25 +2863,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="84" t="s">
-        <v>83</v>
-      </c>
       <c r="C1" s="84" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="83"/>
       <c r="C2" s="87" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" s="86"/>
       <c r="E2" s="86"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="85" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>